<commit_message>
Newest affordability summary spreadsheet
</commit_message>
<xml_diff>
--- a/DATA/PROCESSED/Affordability.xlsx
+++ b/DATA/PROCESSED/Affordability.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walke\OneDrive\Documents\Duke\Masters Project\Shrinking_Cities_MP\DATA\PROCESSED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32557445-95CF-46C2-80A7-F38935460580}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A43DD6-5C1D-450E-9309-95DBECC9ABE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9E8F70ED-9192-4798-993B-B8CCD89841F6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="54">
   <si>
     <t>PWSID</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Chester</t>
+  </si>
+  <si>
+    <t>Focus_City</t>
   </si>
 </sst>
 </file>
@@ -270,7 +273,15 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -430,24 +441,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47FC3FE4-94BC-430C-9BC1-DD50482D0714}" name="Table1" displayName="Table1" ref="A1:K18" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12">
-  <autoFilter ref="A1:K18" xr:uid="{0D1A120F-85D7-48AB-A4D3-644F12D217A3}"/>
-  <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{4F8C4616-09B4-4B62-A830-582F05A63C36}" name="PWSID" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{C9BC8B7F-0D42-432C-AFF7-299C225E3CB0}" name="Name" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{F3C2FDE5-60B1-49B6-93D7-07FE5D458ABC}" name="RateYear" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{C671A65D-1474-499E-82CB-F3ACBA604F51}" name="Monthly_Volume_(gal)" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{F21CB3E3-FB8E-472F-B1F0-86A1FEB5D5F9}" name="Monthly_Cost" dataDxfId="6" dataCellStyle="Currency"/>
-    <tableColumn id="6" xr3:uid="{6A9BB4A4-54EE-4946-9F99-FC06A283AB67}" name="Annual_Cost" dataDxfId="5" dataCellStyle="Currency">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{47FC3FE4-94BC-430C-9BC1-DD50482D0714}" name="Table1" displayName="Table1" ref="A1:L18" totalsRowShown="0" headerRowDxfId="14" dataDxfId="12" headerRowBorderDxfId="13">
+  <autoFilter ref="A1:L18" xr:uid="{0D1A120F-85D7-48AB-A4D3-644F12D217A3}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{4F8C4616-09B4-4B62-A830-582F05A63C36}" name="PWSID" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C9BC8B7F-0D42-432C-AFF7-299C225E3CB0}" name="Name" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{F3C2FDE5-60B1-49B6-93D7-07FE5D458ABC}" name="RateYear" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{C671A65D-1474-499E-82CB-F3ACBA604F51}" name="Monthly_Volume_(gal)" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{F21CB3E3-FB8E-472F-B1F0-86A1FEB5D5F9}" name="Monthly_Cost" dataDxfId="7" dataCellStyle="Currency"/>
+    <tableColumn id="6" xr3:uid="{6A9BB4A4-54EE-4946-9F99-FC06A283AB67}" name="Annual_Cost" dataDxfId="6" dataCellStyle="Currency">
       <calculatedColumnFormula>E2*12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{92601A6B-1CFA-41E9-82C4-4939C9A6B6D2}" name="LQI_2017" dataDxfId="4" dataCellStyle="Currency"/>
-    <tableColumn id="8" xr3:uid="{8DEF86BC-4489-483C-A0D9-C6A84042D9E0}" name="HBI" dataDxfId="3" dataCellStyle="Percent">
+    <tableColumn id="7" xr3:uid="{92601A6B-1CFA-41E9-82C4-4939C9A6B6D2}" name="LQI_2017" dataDxfId="5" dataCellStyle="Currency"/>
+    <tableColumn id="8" xr3:uid="{8DEF86BC-4489-483C-A0D9-C6A84042D9E0}" name="HBI" dataDxfId="4" dataCellStyle="Percent">
       <calculatedColumnFormula>F2/G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{050A8E8D-0AF7-412A-80CD-FA367BD13D38}" name="PPI_2017" dataDxfId="2"/>
-    <tableColumn id="10" xr3:uid="{C688A84A-3CD1-4863-8546-07416EBD892E}" name="Customer_Assistance_Program" dataDxfId="1"/>
-    <tableColumn id="11" xr3:uid="{D2E4AAD8-F155-4F0C-9AF7-A0A9425172E1}" name="notes" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{050A8E8D-0AF7-412A-80CD-FA367BD13D38}" name="PPI_2017" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{C688A84A-3CD1-4863-8546-07416EBD892E}" name="Customer_Assistance_Program" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{E90466BC-98B5-4C86-992F-53F103F86657}" name="Focus_City" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{D2E4AAD8-F155-4F0C-9AF7-A0A9425172E1}" name="notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -750,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0298F258-5C70-448B-AB7B-83AEC142585F}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -767,11 +779,12 @@
     <col min="7" max="7" width="12.81640625" style="6" customWidth="1"/>
     <col min="8" max="8" width="8.7265625" style="2"/>
     <col min="9" max="9" width="10.54296875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="28.7265625" style="2" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="2"/>
+    <col min="10" max="10" width="13.54296875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="11.90625" style="2" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,10 +816,13 @@
         <v>46</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -840,8 +856,11 @@
       <c r="J2" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K2" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -875,11 +894,14 @@
       <c r="J3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -913,8 +935,11 @@
       <c r="J4" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K4" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -948,8 +973,11 @@
       <c r="J5" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K5" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -983,11 +1011,14 @@
       <c r="J6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1021,11 +1052,14 @@
       <c r="J7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1058,8 +1092,11 @@
       <c r="J8" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K8" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -1093,8 +1130,11 @@
       <c r="J9" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K9" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1128,8 +1168,11 @@
       <c r="J10" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K10" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1163,8 +1206,11 @@
       <c r="J11" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1198,8 +1244,11 @@
       <c r="J12" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K12" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -1233,11 +1282,14 @@
       <c r="J13" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="K13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -1271,8 +1323,11 @@
       <c r="J14" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>23</v>
       </c>
@@ -1306,8 +1361,11 @@
       <c r="J15" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K15" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>24</v>
       </c>
@@ -1338,11 +1396,14 @@
       <c r="J16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>26</v>
       </c>
@@ -1376,8 +1437,11 @@
       <c r="J17" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K17" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>28</v>
       </c>
@@ -1409,6 +1473,9 @@
         <v>0.36630000000000001</v>
       </c>
       <c r="J18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K18" s="4" t="s">
         <v>40</v>
       </c>
     </row>

</xml_diff>